<commit_message>
feat: azure services cost updated closed #1
</commit_message>
<xml_diff>
--- a/pricing/cost_Estimations.xlsx
+++ b/pricing/cost_Estimations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Microsoft Azure Estimate</t>
   </si>
@@ -53,7 +53,7 @@
     <t>France Central</t>
   </si>
   <si>
-    <t>Azure Cosmos DB for NoSQL (anciennement Core), Débit provisionné Standard (manuel), Quantité toujours libre activée, Écriture dans une seule région (maître unique) - France Centre (Région d’écriture), 400 RU/s x 40 Heures, 0 Go de stockage transactionnel, Stockage analytique activé, 2 copies d’un stockage sur sauvegarde périodique, Passerelle dédiée activée, 1 nœuds D4s x 40 Heures</t>
+    <t>Azure Cosmos DB for NoSQL (anciennement Core), Débit provisionné Standard (manuel), Quantité toujours libre désactivée, Écriture dans une seule région (maître unique) - France Centre (Région d’écriture), 400 RU/s x 40 Heures, 0 Go de stockage transactionnel, Stockage analytique désactivé, 2 copies d’un stockage sur sauvegarde périodique, Passerelle dédiée non activée</t>
   </si>
   <si>
     <t>Calcul</t>
@@ -63,6 +63,24 @@
   </si>
   <si>
     <t>Niveau Consommation, À l'utilisation, 128 Mo de mémoire, 100 millisecondes de temps d'exécution, 0 exécutions/mo</t>
+  </si>
+  <si>
+    <t>Internet des Objets</t>
+  </si>
+  <si>
+    <t>Logic Apps</t>
+  </si>
+  <si>
+    <t>Charges de travail : Plan de consommation, 0 Exécutions d’actions par jour x 1 jour, Conservation des données de 0Go, 0 Exécutions du connecteur standard par jour x 1 jour, 0 Exécutions du connecteur entreprise par jour x 1 jour ; Environnement de service d’intégration : niveau Premium, 0 Unités de base x 730 Heures, 0 Unités d’échelle x 730 Heures ; Comptes d’intégration : 0 Comptes d’intégration Standard x 730 Heures, 0 Comptes d’intégration de base x 730 Heures.</t>
+  </si>
+  <si>
+    <t>IA + Machine Learning</t>
+  </si>
+  <si>
+    <t>Azure AI services</t>
+  </si>
+  <si>
+    <t>Langage Azure AI, À l'utilisation, Gratuit</t>
   </si>
   <si>
     <t>Support</t>
@@ -89,7 +107,7 @@
     <t>All prices shown are in United States – Dollar ($) USD. This is a summary estimate, not a quote. For up to date pricing information please visit https://azure.microsoft.com/pricing/calculator/</t>
   </si>
   <si>
-    <t>This estimate was created at 12/25/2023 2:09:08 PM UTC.</t>
+    <t>This estimate was created at 12/25/2023 5:15:38 PM UTC.</t>
   </si>
 </sst>
 </file>
@@ -362,7 +380,7 @@
         <v>13</v>
       </c>
       <c r="F4" s="5">
-        <v>16.49</v>
+        <v>1.6</v>
       </c>
       <c r="G4" s="5">
         <v>0</v>
@@ -433,12 +451,18 @@
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="13" t="s">
-        <v>17</v>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
       </c>
-      <c r="E6" s="12"/>
+      <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="F6" s="5">
         <v>0</v>
       </c>
@@ -466,17 +490,27 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="13" t="s">
-        <v>18</v>
+      <c r="A7" s="3" t="s">
+        <v>20</v>
       </c>
-      <c r="E7" s="13" t="s">
-        <v>19</v>
+      <c r="B7" s="3" t="s">
+        <v>21</v>
       </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="C7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0</v>
+      </c>
       <c r="H7" s="7"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -498,17 +532,21 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8">
-      <c r="A8" s="3"/>
+      <c r="A8" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
-      <c r="E8" s="13" t="s">
-        <v>11</v>
+      <c r="E8" s="12"/>
+      <c r="F8" s="5">
+        <v>0</v>
       </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="G8" s="5">
+        <v>0</v>
+      </c>
       <c r="H8" s="7"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -534,10 +572,10 @@
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="13" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
@@ -565,16 +603,14 @@
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="14" t="s">
-        <v>22</v>
+      <c r="D10" s="13" t="s">
+        <v>26</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="15">
-        <v>16.49</v>
+      <c r="E10" s="13" t="s">
+        <v>11</v>
       </c>
-      <c r="G10" s="15">
-        <v>0</v>
-      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
       <c r="H10" s="7"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -599,8 +635,12 @@
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="D11" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>11</v>
+      </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="7"/>
@@ -624,15 +664,19 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12">
-      <c r="A12" s="13" t="s">
-        <v>23</v>
-      </c>
+      <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
+      <c r="D12" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="15">
+        <v>1.6</v>
+      </c>
+      <c r="G12" s="15">
+        <v>0</v>
+      </c>
       <c r="H12" s="7"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -654,15 +698,13 @@
       <c r="Z12" s="1"/>
     </row>
     <row r="13">
-      <c r="A13" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
       <c r="H13" s="7"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -684,15 +726,15 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14">
-      <c r="A14" s="16" t="s">
-        <v>25</v>
+      <c r="A14" s="13" t="s">
+        <v>29</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
       <c r="H14" s="7"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -714,7 +756,9 @@
       <c r="Z14" s="1"/>
     </row>
     <row r="15">
-      <c r="A15" s="16"/>
+      <c r="A15" s="16" t="s">
+        <v>30</v>
+      </c>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
@@ -742,13 +786,15 @@
       <c r="Z15" s="1"/>
     </row>
     <row r="16">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
+      <c r="A16" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
       <c r="H16" s="7"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -770,13 +816,13 @@
       <c r="Z16" s="1"/>
     </row>
     <row r="17">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
       <c r="H17" s="7"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -28325,8 +28371,8 @@
   <mergeCells>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="A16:G16"/>
   </mergeCells>
   <headerFooter/>
 </worksheet>

</xml_diff>